<commit_message>
Complete Part B. Runner and Customer Experience
</commit_message>
<xml_diff>
--- a/8 Week SQL Challenge/Case Study #2 - Pizza Runner/Database Overview.xlsx
+++ b/8 Week SQL Challenge/Case Study #2 - Pizza Runner/Database Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thinkbook\Desktop\Projects\Mentorship-Program\8 Week SQL Challenge\Case Study #2 - Pizza Runner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A72E402-1BEC-4D4C-AACC-E0E0DDC12A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB9D477-212E-49D5-94CB-3ADB0F1F59AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{3E6E71BB-9682-4F39-A5CA-95C68E4FF3D7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>runner_id</t>
   </si>
@@ -163,6 +163,39 @@
   </si>
   <si>
     <t>pizza_toppings</t>
+  </si>
+  <si>
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>FROM</t>
+  </si>
+  <si>
+    <t>WHERE</t>
+  </si>
+  <si>
+    <t>GROUP BY</t>
+  </si>
+  <si>
+    <t>HAVING</t>
+  </si>
+  <si>
+    <t>ORDER BY</t>
+  </si>
+  <si>
+    <t>LIMIT</t>
+  </si>
+  <si>
+    <t>runner</t>
+  </si>
+  <si>
+    <t>avg()</t>
+  </si>
+  <si>
+    <t>What is the successful delivery percentage for each runner?</t>
+  </si>
+  <si>
+    <t>successful_perc</t>
   </si>
 </sst>
 </file>
@@ -178,12 +211,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -309,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -326,6 +365,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1422,10 +1463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B2C79D-BA41-41C2-8985-59B1D5210CAF}">
-  <dimension ref="B1:J38"/>
+  <dimension ref="B1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1439,12 +1480,13 @@
     <col min="8" max="8" width="9.54296875" customWidth="1"/>
     <col min="9" max="9" width="19.7265625" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="13" max="13" width="12.36328125" customWidth="1"/>
-    <col min="14" max="14" width="12.90625" customWidth="1"/>
+    <col min="12" max="12" width="17.26953125" customWidth="1"/>
+    <col min="13" max="13" width="17.1796875" customWidth="1"/>
+    <col min="14" max="14" width="21.81640625" customWidth="1"/>
     <col min="15" max="15" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -1455,7 +1497,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1475,7 +1517,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3" s="3">
         <v>1</v>
       </c>
@@ -1495,7 +1537,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -1515,7 +1557,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -1523,7 +1565,7 @@
         <v>44204</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -1531,7 +1573,7 @@
         <v>44211</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -1539,7 +1581,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1565,14 +1607,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>1</v>
       </c>
       <c r="C11" s="7">
         <v>101</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="16">
         <v>1</v>
       </c>
       <c r="E11" s="7"/>
@@ -1587,14 +1629,14 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <v>2</v>
       </c>
       <c r="C12" s="7">
         <v>101</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="16">
         <v>1</v>
       </c>
       <c r="E12" s="7"/>
@@ -1609,14 +1651,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <v>3</v>
       </c>
       <c r="C13" s="7">
         <v>102</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="16">
         <v>1</v>
       </c>
       <c r="E13" s="7"/>
@@ -1631,7 +1673,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <v>3</v>
       </c>
@@ -1653,14 +1695,14 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <v>4</v>
       </c>
       <c r="C15" s="7">
         <v>103</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="16">
         <v>1</v>
       </c>
       <c r="E15" s="7">
@@ -1676,15 +1718,21 @@
       <c r="J15" s="14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="L15" t="s">
+        <v>50</v>
+      </c>
+      <c r="M15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <v>4</v>
       </c>
       <c r="C16" s="7">
         <v>103</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="16">
         <v>1</v>
       </c>
       <c r="E16" s="7">
@@ -1700,6 +1748,9 @@
       <c r="J16" s="14" t="s">
         <v>35</v>
       </c>
+      <c r="M16" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
@@ -1732,7 +1783,7 @@
       <c r="C18" s="7">
         <v>104</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="16">
         <v>1</v>
       </c>
       <c r="E18" s="7"/>
@@ -1802,7 +1853,7 @@
       <c r="C21" s="7">
         <v>102</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="16">
         <v>1</v>
       </c>
       <c r="E21" s="7"/>
@@ -1824,7 +1875,7 @@
       <c r="C22" s="7">
         <v>103</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="16">
         <v>1</v>
       </c>
       <c r="E22" s="7">
@@ -1850,7 +1901,7 @@
       <c r="C23" s="7">
         <v>104</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="16">
         <v>1</v>
       </c>
       <c r="E23" s="7"/>
@@ -1866,7 +1917,7 @@
       <c r="C24" s="11">
         <v>104</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="17">
         <v>1</v>
       </c>
       <c r="E24" s="11" t="s">
@@ -1883,6 +1934,9 @@
       <c r="B27" t="s">
         <v>19</v>
       </c>
+      <c r="I27" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B28" s="1" t="s">
@@ -1903,6 +1957,9 @@
       <c r="G28" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="I28" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B29" s="3">
@@ -1921,6 +1978,9 @@
         <v>32</v>
       </c>
       <c r="G29" s="14"/>
+      <c r="I29" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B30" s="3">
@@ -1939,6 +1999,9 @@
         <v>27</v>
       </c>
       <c r="G30" s="14"/>
+      <c r="I30" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B31" s="3">
@@ -1957,6 +2020,9 @@
         <v>20</v>
       </c>
       <c r="G31" s="14"/>
+      <c r="I31" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B32" s="3">
@@ -1975,8 +2041,11 @@
         <v>40</v>
       </c>
       <c r="G32" s="14"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B33" s="3">
         <v>5</v>
       </c>
@@ -1993,8 +2062,11 @@
         <v>15</v>
       </c>
       <c r="G33" s="14"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B34" s="3">
         <v>6</v>
       </c>
@@ -2007,8 +2079,11 @@
       <c r="G34" s="14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B35" s="3">
         <v>7</v>
       </c>
@@ -2026,7 +2101,7 @@
       </c>
       <c r="G35" s="14"/>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B36" s="3">
         <v>8</v>
       </c>
@@ -2044,7 +2119,7 @@
       </c>
       <c r="G36" s="14"/>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B37" s="3">
         <v>9</v>
       </c>
@@ -2058,7 +2133,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B38" s="5">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Complete Case Study #2
</commit_message>
<xml_diff>
--- a/8 Week SQL Challenge/Case Study #2 - Pizza Runner/Database Overview.xlsx
+++ b/8 Week SQL Challenge/Case Study #2 - Pizza Runner/Database Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thinkbook\Desktop\Projects\Mentorship-Program\8 Week SQL Challenge\Case Study #2 - Pizza Runner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB9D477-212E-49D5-94CB-3ADB0F1F59AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDADDF4-8D93-44C8-A21E-BC7B88B36397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{3E6E71BB-9682-4F39-A5CA-95C68E4FF3D7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>runner_id</t>
   </si>
@@ -186,16 +186,10 @@
     <t>LIMIT</t>
   </si>
   <si>
-    <t>runner</t>
-  </si>
-  <si>
-    <t>avg()</t>
-  </si>
-  <si>
-    <t>What is the successful delivery percentage for each runner?</t>
-  </si>
-  <si>
-    <t>successful_perc</t>
+    <t>customer_order_id</t>
+  </si>
+  <si>
+    <t>exclusion_id</t>
   </si>
 </sst>
 </file>
@@ -1463,10 +1457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B2C79D-BA41-41C2-8985-59B1D5210CAF}">
-  <dimension ref="B1:M38"/>
+  <dimension ref="B1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1474,19 +1468,20 @@
     <col min="2" max="2" width="13.36328125" customWidth="1"/>
     <col min="3" max="3" width="18.54296875" customWidth="1"/>
     <col min="4" max="4" width="20.6328125" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" customWidth="1"/>
+    <col min="5" max="5" width="24.26953125" customWidth="1"/>
     <col min="6" max="6" width="19.1796875" customWidth="1"/>
     <col min="7" max="7" width="23.90625" customWidth="1"/>
     <col min="8" max="8" width="9.54296875" customWidth="1"/>
     <col min="9" max="9" width="19.7265625" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="21.54296875" customWidth="1"/>
     <col min="12" max="12" width="17.26953125" customWidth="1"/>
     <col min="13" max="13" width="17.1796875" customWidth="1"/>
     <col min="14" max="14" width="21.81640625" customWidth="1"/>
     <col min="15" max="15" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -1497,7 +1492,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1516,8 +1511,14 @@
       <c r="I2" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="K2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" s="3">
         <v>1</v>
       </c>
@@ -1537,7 +1538,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -1557,7 +1558,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -1565,7 +1566,7 @@
         <v>44204</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -1573,7 +1574,7 @@
         <v>44211</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -1581,7 +1582,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1607,7 +1608,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>1</v>
       </c>
@@ -1629,7 +1630,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <v>2</v>
       </c>
@@ -1651,7 +1652,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <v>3</v>
       </c>
@@ -1673,7 +1674,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <v>3</v>
       </c>
@@ -1695,7 +1696,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <v>4</v>
       </c>
@@ -1718,14 +1719,8 @@
       <c r="J15" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="L15" t="s">
-        <v>50</v>
-      </c>
-      <c r="M15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <v>4</v>
       </c>
@@ -1747,9 +1742,6 @@
       </c>
       <c r="J16" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="M16" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.35">
@@ -1933,9 +1925,6 @@
     <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>19</v>
-      </c>
-      <c r="I27" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.35">
@@ -2153,13 +2142,14 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="6">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>